<commit_message>
Clean up vars and Add Reporting
</commit_message>
<xml_diff>
--- a/data/refunds.xlsx
+++ b/data/refunds.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\RPA\github\refundBot\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A741661-64D9-48CA-9076-5E69806BCA44}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52F7905E-A87A-4EEE-BCDC-96E4F11D2702}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="630" windowWidth="15600" windowHeight="18840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,17 +32,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="84">
   <si>
     <t>YourTicketNumber</t>
   </si>
   <si>
-    <t>AgentID</t>
-  </si>
-  <si>
-    <t>FareType</t>
-  </si>
-  <si>
     <t>Payment_Type</t>
   </si>
   <si>
@@ -55,9 +49,6 @@
     <t>Destination</t>
   </si>
   <si>
-    <t>DeptDate</t>
-  </si>
-  <si>
     <t>Status Code</t>
   </si>
   <si>
@@ -73,55 +64,103 @@
     <t>E3A98987</t>
   </si>
   <si>
-    <t xml:space="preserve">PT434   </t>
-  </si>
-  <si>
-    <t>RTN</t>
-  </si>
-  <si>
     <t xml:space="preserve">Card                </t>
   </si>
   <si>
+    <t>00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Ticket refunded</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
     <t>E3A98988</t>
   </si>
   <si>
+    <t>98</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Refund error</t>
+  </si>
+  <si>
+    <t>2021-12-29 09:25:34</t>
+  </si>
+  <si>
     <t>E3B00190</t>
   </si>
   <si>
+    <t>2021-12-29 09:25:44</t>
+  </si>
+  <si>
     <t>E3B00195</t>
   </si>
   <si>
+    <t>2021-12-29 09:25:55</t>
+  </si>
+  <si>
     <t>E3B00293</t>
   </si>
   <si>
     <t xml:space="preserve">Cash               </t>
   </si>
   <si>
+    <t>02</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Invalid payment type</t>
+  </si>
+  <si>
+    <t>2021-12-29 09:26:06</t>
+  </si>
+  <si>
     <t>E3B00362</t>
   </si>
   <si>
-    <t>SGL</t>
+    <t>03</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Invalid amount</t>
+  </si>
+  <si>
+    <t>2021-12-29 09:26:16</t>
   </si>
   <si>
     <t>X123456</t>
   </si>
   <si>
-    <t xml:space="preserve">FE085    </t>
+    <t>01</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> InvalidTicketNumber</t>
+  </si>
+  <si>
+    <t>2021-12-29 09:26:27</t>
   </si>
   <si>
     <t>P3B48847</t>
   </si>
   <si>
+    <t>2021-12-29 09:26:39</t>
+  </si>
+  <si>
     <t>P3B48848</t>
   </si>
   <si>
+    <t>2021-12-29 09:26:49</t>
+  </si>
+  <si>
+    <t>2021-12-29 09:27:00</t>
+  </si>
+  <si>
     <t>00- Success</t>
   </si>
   <si>
     <t>01 - Invalid Ticket</t>
   </si>
   <si>
-    <t>Invalid Payment Type</t>
+    <t>02 - Invalid Payment Type</t>
   </si>
   <si>
     <t>03 - Invalid Amount</t>
@@ -131,6 +170,120 @@
   </si>
   <si>
     <t>99 - Bot Error</t>
+  </si>
+  <si>
+    <t>CustomerName</t>
+  </si>
+  <si>
+    <t>CustomerAddress</t>
+  </si>
+  <si>
+    <t>Reason</t>
+  </si>
+  <si>
+    <t>John Higgins</t>
+  </si>
+  <si>
+    <t>Neil Hardy</t>
+  </si>
+  <si>
+    <t>Jim Davies</t>
+  </si>
+  <si>
+    <t>Sidney Barrett</t>
+  </si>
+  <si>
+    <t>Kate Crumble</t>
+  </si>
+  <si>
+    <t>Judy Bench</t>
+  </si>
+  <si>
+    <t>Jed Grissom</t>
+  </si>
+  <si>
+    <t>Tom Cotton</t>
+  </si>
+  <si>
+    <t>44 Benchmark Place, Reading, RG30 3HT</t>
+  </si>
+  <si>
+    <t>23 Acacia Av, Bath, BA13 3HS</t>
+  </si>
+  <si>
+    <t>12 Conucopia Way, Bristol BR1 6GH</t>
+  </si>
+  <si>
+    <t>68 Freemason Drive, London, SW12 7EW</t>
+  </si>
+  <si>
+    <t>12 Chalkpit Close, Southampton, SO2 6HP</t>
+  </si>
+  <si>
+    <t>92 Greenacre Avenue, Newcastle, NE2 5TH</t>
+  </si>
+  <si>
+    <t>23 Keep Drive, Aberdeen, AB45 7GB</t>
+  </si>
+  <si>
+    <t>15 Agent Street, Hounslow, HS34 34Y</t>
+  </si>
+  <si>
+    <t>28 Beekeeper Road, Taunton, TA2 6HP</t>
+  </si>
+  <si>
+    <t>Mary Quantum</t>
+  </si>
+  <si>
+    <t>Covid</t>
+  </si>
+  <si>
+    <t>Bognor</t>
+  </si>
+  <si>
+    <t>Newcastle</t>
+  </si>
+  <si>
+    <t>Carlisle</t>
+  </si>
+  <si>
+    <t>Victoria</t>
+  </si>
+  <si>
+    <t>Reading</t>
+  </si>
+  <si>
+    <t>Newbury</t>
+  </si>
+  <si>
+    <t>Doncaster</t>
+  </si>
+  <si>
+    <t>Bournemouth</t>
+  </si>
+  <si>
+    <t>Aberdeen</t>
+  </si>
+  <si>
+    <t>Cardiff</t>
+  </si>
+  <si>
+    <t>G8793984</t>
+  </si>
+  <si>
+    <t>Tim Trubshaw</t>
+  </si>
+  <si>
+    <t>41 Newdenture Av, Blackpool, BA34  34Y</t>
+  </si>
+  <si>
+    <t>Change of plan</t>
+  </si>
+  <si>
+    <t>Sprained Ankle</t>
+  </si>
+  <si>
+    <t>Flying instead</t>
   </si>
 </sst>
 </file>
@@ -140,7 +293,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$]dd/mm/yyyy;@"/>
   </numFmts>
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -287,6 +440,12 @@
       <b/>
       <sz val="12"/>
       <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -633,7 +792,7 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="9"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="29" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="36" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -658,6 +817,11 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="29" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="20" fillId="4" borderId="0" xfId="36" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="4" borderId="0" xfId="36" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="22" fontId="20" fillId="4" borderId="0" xfId="36" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="1" builtinId="30" customBuiltin="1"/>
@@ -994,7 +1158,7 @@
                   <c:v>01 - Invalid Ticket</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Invalid Payment Type</c:v>
+                  <c:v>02 - Invalid Payment Type</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>03 - Invalid Amount</c:v>
@@ -1015,19 +1179,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0</c:v>
@@ -2031,20 +2195,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05048FD4-FE6B-4DFE-B6DC-9425F4DD8CDF}">
-  <dimension ref="A1:L10"/>
+  <dimension ref="A1:L11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2:L10"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17.25" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="9" style="1" customWidth="1"/>
+    <col min="2" max="2" width="14.875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="37.625" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14" style="15" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14" style="15" customWidth="1"/>
     <col min="6" max="6" width="15.5" style="11" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9" style="1" customWidth="1"/>
+    <col min="7" max="7" width="10.875" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="15.5" style="13" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11" style="9" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="39.125" style="2" bestFit="1" customWidth="1"/>
@@ -2057,271 +2222,417 @@
         <v>0</v>
       </c>
       <c r="B1" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="D1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="E1" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="F1" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="14" t="s">
+      <c r="G1" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="10" t="s">
+      <c r="H1" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="I1" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="J1" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="12" t="s">
+      <c r="K1" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="8" t="s">
+      <c r="L1" s="8" t="s">
         <v>8</v>
-      </c>
-      <c r="J1" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="8" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>13</v>
+        <v>49</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>14</v>
+        <v>57</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="E2" s="15">
         <v>4</v>
       </c>
       <c r="F2" s="11">
-        <v>44034.549434988403</v>
-      </c>
-      <c r="G2" s="1">
-        <v>33023</v>
-      </c>
-      <c r="H2" s="13">
-        <v>44295</v>
+        <v>44399.549432870372</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="H2" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="I2" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="J2" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="K2" s="18">
+        <v>44559.392627314817</v>
+      </c>
+      <c r="L2" s="16" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>13</v>
+        <v>66</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>14</v>
+        <v>58</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="E3" s="15">
         <v>4</v>
       </c>
       <c r="F3" s="11">
-        <v>44034.555427048603</v>
-      </c>
-      <c r="G3" s="1">
-        <v>57366</v>
-      </c>
-      <c r="H3" s="13">
-        <v>44295</v>
+        <v>44399.555428240739</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="H3" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="I3" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="J3" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="K3" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="L3" s="16" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>13</v>
+        <v>55</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>14</v>
+        <v>59</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="E4" s="15">
         <v>17.600000000000001</v>
       </c>
       <c r="F4" s="11">
-        <v>44130.444795335701</v>
-      </c>
-      <c r="G4" s="1">
-        <v>33023</v>
-      </c>
-      <c r="H4" s="13">
-        <v>44244</v>
+        <v>44495.444791666669</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="H4" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="I4" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="J4" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="K4" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="L4" s="16" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>13</v>
+        <v>50</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>14</v>
+        <v>60</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="E5" s="15">
         <v>9.1999999999999993</v>
       </c>
       <c r="F5" s="11">
-        <v>44130.562278506899</v>
-      </c>
-      <c r="G5" s="1">
-        <v>33023</v>
-      </c>
-      <c r="H5" s="13">
-        <v>44244</v>
+        <v>44495.562280092592</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="H5" s="13" t="s">
+        <v>82</v>
+      </c>
+      <c r="I5" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="J5" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="K5" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="L5" s="16" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>13</v>
+        <v>51</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>14</v>
+        <v>61</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="E6" s="15">
         <v>57.7</v>
       </c>
       <c r="F6" s="11">
-        <v>44152.329589039298</v>
-      </c>
-      <c r="G6" s="1">
-        <v>57366</v>
-      </c>
-      <c r="H6" s="13">
-        <v>44255</v>
+        <v>44517.329583333332</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="H6" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="I6" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="J6" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="K6" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="L6" s="16" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="B7" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" s="15">
+        <v>1000000</v>
+      </c>
+      <c r="F7" s="11">
+        <v>44525.528923611113</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="H7" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="I7" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="J7" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="K7" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="L7" s="16" t="s">
         <v>13</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E7" s="15">
-        <v>6756567</v>
-      </c>
-      <c r="F7" s="11">
-        <v>44160.528927893502</v>
-      </c>
-      <c r="G7" s="1">
-        <v>76122</v>
-      </c>
-      <c r="H7" s="13">
-        <v>44246</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>24</v>
+        <v>52</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>22</v>
+        <v>63</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="E8" s="15">
         <v>30.3</v>
       </c>
       <c r="F8" s="11">
-        <v>44179.481161770796</v>
-      </c>
-      <c r="G8" s="1">
-        <v>33023</v>
-      </c>
-      <c r="H8" s="13">
-        <v>44245</v>
+        <v>44544.481157407405</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="H8" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="I8" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="J8" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="K8" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="L8" s="16" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>13</v>
+        <v>53</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>14</v>
+        <v>65</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="E9" s="15">
         <v>19.5</v>
       </c>
       <c r="F9" s="11">
-        <v>44201.391748958296</v>
-      </c>
-      <c r="G9" s="1">
-        <v>33343</v>
-      </c>
-      <c r="H9" s="13">
-        <v>44243</v>
+        <v>44566.391747685186</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="H9" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="I9" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="J9" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="K9" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="L9" s="16" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>26</v>
+        <v>37</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>13</v>
+        <v>54</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>14</v>
+        <v>64</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="E10" s="15">
         <v>18.3</v>
       </c>
       <c r="F10" s="11">
-        <v>44201.3918086458</v>
-      </c>
-      <c r="G10" s="1">
-        <v>33343</v>
-      </c>
-      <c r="H10" s="13">
-        <v>44243</v>
+        <v>44566.391805555555</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="H10" s="13" t="s">
+        <v>83</v>
+      </c>
+      <c r="I10" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="J10" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="K10" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="L10" s="16" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E11" s="15">
+        <v>23.56</v>
+      </c>
+      <c r="F11" s="11">
+        <v>44625.391805555555</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="H11" s="13" t="s">
+        <v>81</v>
+      </c>
+      <c r="I11" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="J11" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="K11" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="L11" s="16" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -2335,58 +2646,58 @@
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.375" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.75" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="18.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>27</v>
+        <v>40</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>28</v>
+        <v>41</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>29</v>
+        <v>42</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>30</v>
+        <v>43</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>31</v>
+        <v>44</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>32</v>
+        <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="4">
         <f>COUNTIFS(Tickets!I1:I990, "00")</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="B2" s="4">
         <f>COUNTIFS(Tickets!I1:I990, "01")</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C2" s="4">
         <f>COUNTIFS(Tickets!I1:I990, "02")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D2" s="4">
         <f>COUNTIFS(Tickets!I1:I990, "03")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E2" s="4">
         <f>COUNTIFS(Tickets!I1:J990, "98")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F2" s="4">
         <f>COUNTIFS(Tickets!I1:K990, "99")</f>

</xml_diff>